<commit_message>
added 3d overlay scatter plots
</commit_message>
<xml_diff>
--- a/graphics.xlsx
+++ b/graphics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pat\Documents\patfiles\python_related\explorations\earthquakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF66C55-5697-49A5-B15E-C5D705EBC29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC6A86-9058-4317-AE70-99F60AF3036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13440" xr2:uid="{7E2BA61D-7775-4C85-B267-F2EFF89C6DD4}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,15 +333,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -360,8 +356,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="647700" y="933450"/>
-          <a:ext cx="1905000" cy="495300"/>
+          <a:off x="885825" y="1028700"/>
+          <a:ext cx="1343025" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -398,37 +394,8 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>great circle</a:t>
+            <a:t>haversine distance</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>km</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> betweeen quake and fracking site</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1488,15 +1455,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
+      <xdr:colOff>171449</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>542924</xdr:colOff>
+      <xdr:colOff>371474</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1511,7 +1478,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2171699" y="1276350"/>
+          <a:off x="2000249" y="1304925"/>
           <a:ext cx="809625" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1546,7 +1513,7 @@
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>dist</a:t>
+            <a:t>linear dist</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -2005,7 +1972,7 @@
   <dimension ref="J3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>